<commit_message>
Add code for led dot points Moved silk coordinate to avoid via
</commit_message>
<xml_diff>
--- a/BOM_BaseBoard.xlsx
+++ b/BOM_BaseBoard.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Minori Takao\Dropbox\Dev\KiCad\NixieClockKit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtakao\Dropbox\Dev\KiCad\NixieClockKit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="8904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22989" windowHeight="8906"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bom!$A$1:$G$31</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="102">
   <si>
     <t>Reference</t>
   </si>
@@ -346,11 +349,87 @@
     </rPh>
     <phoneticPr fontId="18"/>
   </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>socket</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1x4</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1x5</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1x12</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>1x5</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2x3</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>2x4</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>total 47</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>DIP28 socket</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ok</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>DIP16 socket</t>
+    <phoneticPr fontId="18"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1058,7 +1137,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1095,11 +1174,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1455,545 +1537,750 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" customWidth="1"/>
-    <col min="3" max="3" width="44.59765625" customWidth="1"/>
-    <col min="4" max="4" width="26.8984375" customWidth="1"/>
-    <col min="6" max="6" width="45.296875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="5" max="5" width="26.92578125" customWidth="1"/>
+    <col min="7" max="7" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="3">
-        <v>250</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="6">
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C12" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E12" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="6">
+      <c r="F12" s="6">
         <v>20</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G12" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6">
+        <v>10</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="6">
+        <v>250</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="B14" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="6">
+        <v>5</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="6">
+        <v>5</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="6">
+        <v>4</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="6">
+        <v>5</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="6">
+        <v>5</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="6">
+        <v>5</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C21" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="6">
+      <c r="F21" s="6">
         <v>14</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="6">
-        <v>5</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="6">
-        <v>5</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="6">
-        <v>5</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="6">
-        <v>30</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="6">
-        <v>5</v>
-      </c>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="6">
-        <v>5</v>
-      </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="6">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1</v>
-      </c>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="6">
-        <v>80</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="6">
-        <v>90</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A22" t="s">
         <v>43</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="6">
-        <v>200</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>46</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="6">
+      <c r="F22" s="6">
         <v>200</v>
       </c>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G22" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.65">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="6">
+        <v>200</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="6">
         <v>31</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="6">
+      <c r="D24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="6">
+        <v>90</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="B25" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A26" s="6"/>
+      <c r="B26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="14">
+        <v>50</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="6">
+        <v>31</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="6">
+        <v>80</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="11">
+        <v>30</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="6">
+        <f>SUM(F3:F28)</f>
+        <v>972</v>
+      </c>
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A30" s="9"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="A31" s="9"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="12">
+        <f>SUM(F28:F30)</f>
+        <v>1002</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.65">
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>8</v>
+      </c>
+      <c r="G35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.65">
+      <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.65">
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.65">
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.65">
+      <c r="C39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39">
         <v>1</v>
       </c>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="F39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.65">
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.65">
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.65">
+      <c r="C44" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="G44">
         <v>48</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="6">
-        <v>4</v>
-      </c>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="11">
-        <f>SUM(E2:E25)</f>
-        <v>923</v>
-      </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="9"/>
-      <c r="B28" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" s="12">
-        <v>50</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29" s="9"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="13">
-        <f>SUM(E26:E28)</f>
-        <v>973</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>82</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G31">
+    <sortState ref="A2:G29">
+      <sortCondition ref="B1:B29"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>